<commit_message>
Agregué el suavizado del OBS501-SS a los gráficos.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191210_Muelle/ECO_FLNTUProcessed/RdP_20191210_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191210_Muelle/ECO_FLNTUProcessed/RdP_20191210_ECO-FLNTU.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,8 +21,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -61,22 +61,22 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -862,7 +862,7 @@
       <c r="L11" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -983,7 +983,7 @@
       <c r="C11" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1104,7 +1104,7 @@
       <c r="C11" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1225,7 +1225,7 @@
       <c r="C11" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3060,6 +3060,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agregué los gráficos de clorofila.
</commit_message>
<xml_diff>
--- a/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191210_Muelle/ECO_FLNTUProcessed/RdP_20191210_ECO-FLNTU.xlsx
+++ b/FLNTU/Base de datos/Datos/regions/RdP/RdP_20191210_Muelle/ECO_FLNTUProcessed/RdP_20191210_ECO-FLNTU.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Stations_Mean" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Stations_Std" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Stations_CV" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="ECOContSmooth1min" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="stationInfo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stations_Mean" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stations_Std" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Stations_CV" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ECOContSmooth1min" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>